<commit_message>
A1#111AGFAHEALTHC-AGFA GEVAERT SPA-ELEFANTE.NET-2 e Elefante_Web-1
A1#111AGFAHEALTHC-AGFA GEVAERT SPA-ELEFANTE.NET-2 e Elefante_Web-1
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111AGFAHEALTHC/AGFA_GEVAERT_SPA/Elefante_Web/1/report-checklist.xlsx
+++ b/GATEWAY/A1#111AGFAHEALTHC/AGFA_GEVAERT_SPA/Elefante_Web/1/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Manuali\Common\IntegrazioneFSE-ConfidentialityCode\FSE 2.0\REPOSITORY\it-fse-accreditamento\GATEWAY\A1#111AGFAHEALTHC\AGFA_GEVAERT_SPA\Elefante_Web\1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TMP_APPOGGIO\FSE2.0\ELEFANTE_WEB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21038A56-F7AE-4888-A274-173AA3B84815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2FF07B-5830-4322-83EB-99271CDC5E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -522,12 +522,6 @@
     <t>RAZIONALE DI APPLICABILITA' - ALTRO</t>
   </si>
   <si>
-    <t xml:space="preserve"> PRESENTE CODA DI RETRY AUTOMATICA PER L'INVIO DEL DOCUMENTO AL FSE A SEGUITO DELLA RISOLUZIONE DELL'ERRORE (SI/NO)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> INVIO MANUALE DEL DOCUMENTO AL FSE A SEGUITO DELLA RISOLUZIONE DELL'ERRORE (SI/NO)</t>
-  </si>
-  <si>
     <t>Razionale di Applicabilità</t>
   </si>
   <si>
@@ -550,10 +544,6 @@
   </si>
   <si>
     <t>Altro (specificare)</t>
-  </si>
-  <si>
-    <t>Per questo caso di test è richiesta la sola descrizione del comportamento a fronte di un timeout, da inserire nelle colonne relative a:
-"ERRORE BLOCCANTE (SI/NO)", "ERRORE VISIBILE A UTENTE (SI/NO)", "MESSAGGIO DI ERRORE", "GESTITO IN BACKOFFICE (SI/NO)", " PRESENTE CODA DI RETRY AUTOMATICA PER L'INVIO DEL DOCUMENTO AL FSE A SEGUITO DELLA RISOLUZIONE DELL'ERRORE (SI/NO)",  "INVIO MANUALE DEL DOCUMENTO AL FSE A SEGUITO DELLA RISOLUZIONE DELL'ERRORE (SI/NO)", "GESTIONE ERRORE".</t>
   </si>
   <si>
     <t>Versione:</t>
@@ -576,6 +566,246 @@
     </r>
   </si>
   <si>
+    <t>5) Se il test NON è applicabile la colonna APPLICABILITA' riporterà NO e dovrà essere compilata esclusivamente la colonna RAZIONALE DI APPLICABILITA' con le motivazioni per cui il test non è applicabile. Il campo è valorizzabile tramite selezione da menù a tendina (campo/sezione non gestito/a in modo strutturato dall’applicativo;c ampo obbligatorio; campo valorizzato di default; campo valorizzato in automatico tramite dati recuperati da servizi esterni; campo valorizzabile tramite selezione da un set di valori ammessi; l’applicativo effettua controlli preventivi sul dato inserito; altro (specificare)). Nel caso in cui si selezioni l'opzione "Altro (specificare)" è necessario compilare la colonna RAZIONALE DI "APPLICABILITA' - ALTRO" con le motivazioni per le quali il test non è applicabile.</t>
+  </si>
+  <si>
+    <t>6) La colonna TEST AUTOCERTIFICATO non deve mai essere compilata dal fornitore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Necessario compilare sempre le righe 2,3,4,5 con rispettivamente:
+Nome fornitore dell'applicativo
+nome applicazione: subject_application_id
+Nome fornitore: subject_application_vendor
+versione applicazione: subject_application_version
+</t>
+  </si>
+  <si>
+    <t>RAP</t>
+  </si>
+  <si>
+    <t>TIPO DOCUMENTO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 20" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>448, 449</t>
+  </si>
+  <si>
+    <t>450, 451</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>454, 455</t>
+  </si>
+  <si>
+    <t>456, 457</t>
+  </si>
+  <si>
+    <t>458, 459</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT24</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT25</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 24" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 25" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 26" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT26_KO</t>
+  </si>
+  <si>
+    <t>4, 452</t>
+  </si>
+  <si>
+    <t>417, 418, 419, 460</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT24_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 24" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT27_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 27" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>29,37,45,64,66,67,68,69,70,71,72,73,74, 467</t>
+  </si>
+  <si>
+    <t>33,41,49,95,97,98,99,100,101,102,103,104,105,106, 464</t>
+  </si>
+  <si>
+    <t>34,42,50,108,110,111,112,113,114,115,116,117,118,119,120,121, 465</t>
+  </si>
+  <si>
+    <t>35,43,51,123,125,126,127,128,129,130,131,132,133,134,135,136,137,138,139,140,141,142,143,144,145,146, 463</t>
+  </si>
+  <si>
+    <t>30,38,46,175,177,178,179,180,181,182,183,184,185,186,187,188,189,190, 469</t>
+  </si>
+  <si>
+    <t>423,424,425,427,428,429,430,431,432,433,434,435,436,437,438,439,440,441,442,443,448,449, 470</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT25</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Referto Radiologia dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 25" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>3) Nel caso in cui tra le tipologie documentali oggetto di accreditamento per l'applicativo figurino PSS, RAP, RAD, RSA, LDO, LAB, VPS, SING_VACC, CERT_VACC i relativi casi di test con id 444, 417, 418, 460, 448, 450, 452,454, 456, 457, 458, 471 che recepiscono quanto previsto dal Decreto 07 settembre 2023, devono essere obbligatoriamente eseguiti e compilati (la colonna APPLICABILITA' deve essere valorizzata con SI)</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT26</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Referto Radiologia dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 26" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>471, 472</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT28_KO</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT27_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.  
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 27" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 28" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>28,36,44,53,55,56,57,59,60,61,62, 466, 473</t>
+  </si>
+  <si>
+    <t>31,39,47,76,78,79,80,81,83,84,85,86,87,88,89,90,91,92,93, 462, 474</t>
+  </si>
+  <si>
+    <t>32,40,48,152,154,155,156,157,159,160,161,162,163,164,165,166,167,168,169, 461, 468, 475</t>
+  </si>
+  <si>
+    <t>8.2.6.1</t>
+  </si>
+  <si>
+    <t>Per questo caso di test è richiesta la sola descrizione del comportamento a fronte di un timeout, da inserire nelle colonne relative a:
+"ERRORE BLOCCANTE (SI/NO)", "ERRORE VISIBILE A UTENTE (SI/NO)", "MESSAGGIO DI ERRORE", "GESTITO IN BACKOFFICE (SI/NO)", " PRESENTE CODA DI RETRY AUTOMATICA PER L'INVIO DEL DOCUMENTO AL FSE SERVIZIO DI VALIDAZIONE DEL GATEWAY A SEGUITO DELLA RISOLUZIONE DELL'ERRORE (SI/NO)",  "INVIO MANUALE DEL DOCUMENTO AL FSE A SEGUITO DELLA RISOLUZIONE DELL'ERRORE (SI/NO)", "GESTIONE ERRORE".</t>
+  </si>
+  <si>
     <t>4) Se il test è applicabile la colonna APPLICABILITA' deve essere compilata con SI e dovranno essere valorizzate:
     DATA ESECUZIONE, 
     TIMESTAMP, 
@@ -586,289 +816,59 @@
     MESSAGGIO DI ERRORE da compilare con il messaggio di errore visualizzato dall’applicativo, solo per i casi KO (ovvero con colonna CASO OK / KO= KO) e per i casi di test di TIMEOUT visibili all'utente (colonna ERRORE VISIBILE A UTENTE (SI/NO)=SI)
     GESTITO IN BACKOFFICE (SI/NO) da compilare solo per i casi KO (ovvero con colonna CASO OK / KO= KO) e per i casi di test di TIMEOUT,
     PRESENTE CODA DI RETRY AUTOMATICA PER L'INVIO DEL DOCUMENTO A FSE A SEGUITO DELLA RISOLUZIONE DELL'ERRORE (SI/NO) da compilare solo per i casi KO (ovvero con colonna CASO OK / KO= KO) e per i casi di test di TIMEOUT,
-   INVIO MANUALE DEL DOCUMENTO AL FSE A SEGUITO DELLA RISOLUZIONE DELL'ERRORE (SI/NO) da compilare solo per i casi KO  (ovvero con colonna CASO OK / KO= KO) e per i casi di test di TIMEOUT,
+  INVIO MANUALE DEL DOCUMENTO AL FSE SERVIZIO DI VALIDAZIONE DEL GATEWAY A SEGUITO DELLA RISOLUZIONE DELL'ERRORE (SI/NO) da compilare solo per i casi KO  (ovvero con colonna CASO OK / KO= KO) e per i casi di test di TIMEOUT,
     GESTIONE ERRORE da compilare con la procedura che viene adottata per la gestione dell'errore, solo per i casi KO (ovvero con CASO OK / KO= KO) e per i casi di test di TIMEOUT,  specificando le modalità di invio del documento clinico al FSE a seguito della correzione dell'errore e chiarendo se è possibile per l'utente (medico) proseguire con il processo e produrre il documento. Esclusivamente per i casi di test di TIMEOUT, qualora non fosse prevista una coda di retry e la gestione dell'errore non fossa gestita da un operatore di backoffice, indicare le modalità attraverso cui è reso esplicito all’utente (medico) di effettuare nuovi tentativi di invio verso il FSE fino al ripristino del servizio di validazione.</t>
   </si>
   <si>
-    <t>5) Se il test NON è applicabile la colonna APPLICABILITA' riporterà NO e dovrà essere compilata esclusivamente la colonna RAZIONALE DI APPLICABILITA' con le motivazioni per cui il test non è applicabile. Il campo è valorizzabile tramite selezione da menù a tendina (campo/sezione non gestito/a in modo strutturato dall’applicativo;c ampo obbligatorio; campo valorizzato di default; campo valorizzato in automatico tramite dati recuperati da servizi esterni; campo valorizzabile tramite selezione da un set di valori ammessi; l’applicativo effettua controlli preventivi sul dato inserito; altro (specificare)). Nel caso in cui si selezioni l'opzione "Altro (specificare)" è necessario compilare la colonna RAZIONALE DI "APPLICABILITA' - ALTRO" con le motivazioni per le quali il test non è applicabile.</t>
-  </si>
-  <si>
-    <t>6) La colonna TEST AUTOCERTIFICATO non deve mai essere compilata dal fornitore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) Necessario compilare sempre le righe 2,3,4,5 con rispettivamente:
-Nome fornitore dell'applicativo
-nome applicazione: subject_application_id
-Nome fornitore: subject_application_vendor
-versione applicazione: subject_application_version
-</t>
-  </si>
-  <si>
-    <t>RAP</t>
-  </si>
-  <si>
-    <t>TIPO DOCUMENTO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 20" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>448, 449</t>
-  </si>
-  <si>
-    <t>450, 451</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>454, 455</t>
-  </si>
-  <si>
-    <t>456, 457</t>
-  </si>
-  <si>
-    <t>458, 459</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT24</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT25</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 24" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 25" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 26" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT26_KO</t>
-  </si>
-  <si>
-    <t>4, 452</t>
-  </si>
-  <si>
-    <t>417, 418, 419, 460</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RAD_CT24_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 24" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT27_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 27" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>29,37,45,64,66,67,68,69,70,71,72,73,74, 467</t>
-  </si>
-  <si>
-    <t>33,41,49,95,97,98,99,100,101,102,103,104,105,106, 464</t>
-  </si>
-  <si>
-    <t>34,42,50,108,110,111,112,113,114,115,116,117,118,119,120,121, 465</t>
-  </si>
-  <si>
-    <t>35,43,51,123,125,126,127,128,129,130,131,132,133,134,135,136,137,138,139,140,141,142,143,144,145,146, 463</t>
-  </si>
-  <si>
-    <t>30,38,46,175,177,178,179,180,181,182,183,184,185,186,187,188,189,190, 469</t>
-  </si>
-  <si>
-    <t>423,424,425,427,428,429,430,431,432,433,434,435,436,437,438,439,440,441,442,443,448,449, 470</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RAD_CT25</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
-Il Documento CDA2 Referto Radiologia dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 25" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>3) Nel caso in cui tra le tipologie documentali oggetto di accreditamento per l'applicativo figurino PSS, RAP, RAD, RSA, LDO, LAB, VPS, SING_VACC, CERT_VACC i relativi casi di test con id 444, 417, 418, 460, 448, 450, 452,454, 456, 457, 458, 471 che recepiscono quanto previsto dal Decreto 07 settembre 2023, devono essere obbligatoriamente eseguiti e compilati (la colonna APPLICABILITA' deve essere valorizzata con SI)</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RAD_CT26</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
-Il Documento CDA2 Referto Radiologia dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 26" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>471, 472</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT28_KO</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RAD_CT27_KO</t>
-  </si>
-  <si>
-    <t>8.2.6</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.  
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 27" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 28" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>28,36,44,53,55,56,57,59,60,61,62, 466, 473</t>
-  </si>
-  <si>
-    <t>31,39,47,76,78,79,80,81,83,84,85,86,87,88,89,90,91,92,93, 462, 474</t>
-  </si>
-  <si>
-    <t>32,40,48,152,154,155,156,157,159,160,161,162,163,164,165,166,167,168,169, 461, 468, 475</t>
+    <t>PRESENTE CODA DI RETRY AUTOMATICA PER L'INVIO DEL DOCUMENTO AL SERVIZIO DI VALIDAZIONE DEL GATEWAY A SEGUITO DELLA RISOLUZIONE DELL'ERRORE (SI/NO)</t>
+  </si>
+  <si>
+    <t>INVIO MANUALE DEL DOCUMENTO AL SERVIZIO DI VALIDAZIONE DEL GATEWAY A SEGUITO DELLA RISOLUZIONE DELL'ERRORE (SI/NO)</t>
+  </si>
+  <si>
+    <t>subject_application_id: Elefante Web</t>
   </si>
   <si>
     <t>subject_application_vendor: AGFA GEVAERT SPA</t>
   </si>
   <si>
+    <t>subject_application_version: 1</t>
+  </si>
+  <si>
+    <t>2025-09-11T11:58:13Z</t>
+  </si>
+  <si>
+    <t>2025-09-11T12:00:54Z</t>
+  </si>
+  <si>
+    <t>2025-09-10T17:42:40Z</t>
+  </si>
+  <si>
+    <t>594136cba030d46828bd967da5c48e95</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.4.4.206325ee3da836fa543317806c03aa2e5694ddecb397d85fb3f535219a6375af.a8015a2402^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>614f7dc05749744e42f33be8ca20dec5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.4.4.8429b207eecb404630e61e00214a41094a28f0cd98cf6f443dc5ed17b5508781.a6aaa6a183^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Errore nella validazione del documento Richiesta annullata: Timeout dell'operazione</t>
   </si>
   <si>
     <t>Errore viene riportato all'utente che puo' riprovare operazione di invio</t>
   </si>
   <si>
+    <t>2025-09-10T17:08:22Z</t>
+  </si>
+  <si>
+    <t>Nella sezione "Storia Clinica", l'applicativo gestisce solo la parte testuale (tag &lt;text&gt;) e non gestisce la sotto-sezione "entry".</t>
+  </si>
+  <si>
     <t>AGFA GEVAERT SPA</t>
-  </si>
-  <si>
-    <t>Nella sezione "Storia Clinica", l'applicativo gestisce solo la parte testuale (tag &lt;text&gt;) e non gestisce la sotto-sezione "entry".</t>
-  </si>
-  <si>
-    <t>subject_application_id: Elefante Web</t>
-  </si>
-  <si>
-    <t>subject_application_version: 1</t>
-  </si>
-  <si>
-    <t>2025-09-10T17:42:40Z</t>
-  </si>
-  <si>
-    <t>2025-09-10T17:08:22Z</t>
-  </si>
-  <si>
-    <t>594136cba030d46828bd967da5c48e95</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.206325ee3da836fa543317806c03aa2e5694ddecb397d85fb3f535219a6375af.a8015a2402^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>614f7dc05749744e42f33be8ca20dec5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.8429b207eecb404630e61e00214a41094a28f0cd98cf6f443dc5ed17b5508781.a6aaa6a183^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-09-11T11:58:13Z</t>
-  </si>
-  <si>
-    <t>2025-09-11T12:00:54Z</t>
   </si>
 </sst>
 </file>
@@ -1029,7 +1029,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1338,21 +1338,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1471,10 +1462,6 @@
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1486,9 +1473,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal 2" xfId="1" xr:uid="{565105C8-FFD6-432C-8B2E-BD1D172FCD26}"/>
@@ -1790,8 +1778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1807,7 +1795,7 @@
     </row>
     <row r="2" spans="1:1" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
@@ -1817,22 +1805,22 @@
     </row>
     <row r="4" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="300" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>116</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -1930,7 +1918,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2938,11 +2926,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W615"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="O13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2988,10 +2976,10 @@
         <v>12</v>
       </c>
       <c r="B2" s="45"/>
-      <c r="C2" s="46" t="s">
-        <v>186</v>
-      </c>
-      <c r="D2" s="47"/>
+      <c r="C2" s="53" t="s">
+        <v>197</v>
+      </c>
+      <c r="D2" s="54"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -3012,12 +3000,12 @@
       <c r="W2" s="9"/>
     </row>
     <row r="3" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="54" t="s">
-        <v>188</v>
+      <c r="B3" s="47"/>
+      <c r="C3" s="52" t="s">
+        <v>183</v>
       </c>
       <c r="D3" s="45"/>
       <c r="F3" s="6"/>
@@ -3040,10 +3028,10 @@
       <c r="W3" s="9"/>
     </row>
     <row r="4" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="50"/>
-      <c r="B4" s="51"/>
-      <c r="C4" s="54" t="s">
-        <v>183</v>
+      <c r="A4" s="48"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="52" t="s">
+        <v>184</v>
       </c>
       <c r="D4" s="45"/>
       <c r="E4" s="4"/>
@@ -3067,10 +3055,10 @@
       <c r="W4" s="9"/>
     </row>
     <row r="5" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="54" t="s">
-        <v>189</v>
+      <c r="A5" s="50"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="52" t="s">
+        <v>185</v>
       </c>
       <c r="D5" s="45"/>
       <c r="F5" s="6"/>
@@ -3208,10 +3196,10 @@
         <v>28</v>
       </c>
       <c r="Q9" s="20" t="s">
-        <v>102</v>
+        <v>181</v>
       </c>
       <c r="R9" s="20" t="s">
-        <v>103</v>
+        <v>182</v>
       </c>
       <c r="S9" s="20" t="s">
         <v>29</v>
@@ -3253,7 +3241,7 @@
         <v>100</v>
       </c>
       <c r="K10" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L10" s="35"/>
       <c r="M10" s="35"/>
@@ -3294,7 +3282,7 @@
         <v>100</v>
       </c>
       <c r="K11" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L11" s="35"/>
       <c r="M11" s="35"/>
@@ -3335,7 +3323,7 @@
         <v>100</v>
       </c>
       <c r="K12" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L12" s="35"/>
       <c r="M12" s="35"/>
@@ -3376,7 +3364,7 @@
         <v>100</v>
       </c>
       <c r="K13" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L13" s="35"/>
       <c r="M13" s="35"/>
@@ -3407,13 +3395,13 @@
         <v>52</v>
       </c>
       <c r="E14" s="40" t="s">
-        <v>112</v>
+        <v>179</v>
       </c>
       <c r="F14" s="34">
         <v>45911</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="H14" s="34"/>
       <c r="I14" s="39"/>
@@ -3429,7 +3417,7 @@
         <v>51</v>
       </c>
       <c r="O14" s="35" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="P14" s="35" t="s">
         <v>100</v>
@@ -3441,7 +3429,7 @@
         <v>51</v>
       </c>
       <c r="S14" s="35" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="T14" s="35" t="s">
         <v>98</v>
@@ -3466,13 +3454,13 @@
         <v>53</v>
       </c>
       <c r="E15" s="40" t="s">
-        <v>112</v>
+        <v>179</v>
       </c>
       <c r="F15" s="34">
         <v>45911</v>
       </c>
       <c r="G15" s="41" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="H15" s="34"/>
       <c r="I15" s="39"/>
@@ -3488,7 +3476,7 @@
         <v>51</v>
       </c>
       <c r="O15" s="35" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="P15" s="35" t="s">
         <v>100</v>
@@ -3500,7 +3488,7 @@
         <v>51</v>
       </c>
       <c r="S15" s="35" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="T15" s="35" t="s">
         <v>98</v>
@@ -3525,7 +3513,7 @@
         <v>54</v>
       </c>
       <c r="E16" s="40" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F16" s="34"/>
       <c r="G16" s="34"/>
@@ -3535,7 +3523,7 @@
         <v>100</v>
       </c>
       <c r="K16" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L16" s="35"/>
       <c r="M16" s="35"/>
@@ -3576,7 +3564,7 @@
         <v>100</v>
       </c>
       <c r="K17" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L17" s="35"/>
       <c r="M17" s="35"/>
@@ -3607,7 +3595,7 @@
         <v>57</v>
       </c>
       <c r="E18" s="40" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="34"/>
@@ -3617,7 +3605,7 @@
         <v>100</v>
       </c>
       <c r="K18" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L18" s="35"/>
       <c r="M18" s="35"/>
@@ -3648,7 +3636,7 @@
         <v>58</v>
       </c>
       <c r="E19" s="40" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="34"/>
@@ -3658,7 +3646,7 @@
         <v>100</v>
       </c>
       <c r="K19" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L19" s="35"/>
       <c r="M19" s="35"/>
@@ -3689,7 +3677,7 @@
         <v>59</v>
       </c>
       <c r="E20" s="40" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="34"/>
@@ -3699,7 +3687,7 @@
         <v>100</v>
       </c>
       <c r="K20" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L20" s="35"/>
       <c r="M20" s="35"/>
@@ -3740,7 +3728,7 @@
         <v>100</v>
       </c>
       <c r="K21" s="35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L21" s="35"/>
       <c r="M21" s="35"/>
@@ -3781,7 +3769,7 @@
         <v>100</v>
       </c>
       <c r="K22" s="35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L22" s="35"/>
       <c r="M22" s="35"/>
@@ -3812,7 +3800,7 @@
         <v>64</v>
       </c>
       <c r="E23" s="40" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="34"/>
@@ -3822,7 +3810,7 @@
         <v>100</v>
       </c>
       <c r="K23" s="35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L23" s="35"/>
       <c r="M23" s="35"/>
@@ -3853,7 +3841,7 @@
         <v>65</v>
       </c>
       <c r="E24" s="40" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="34"/>
@@ -3863,7 +3851,7 @@
         <v>100</v>
       </c>
       <c r="K24" s="35" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L24" s="35"/>
       <c r="M24" s="35"/>
@@ -3894,7 +3882,7 @@
         <v>66</v>
       </c>
       <c r="E25" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F25" s="34"/>
       <c r="G25" s="34"/>
@@ -3904,7 +3892,7 @@
         <v>100</v>
       </c>
       <c r="K25" s="35" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L25" s="35"/>
       <c r="M25" s="35"/>
@@ -3935,7 +3923,7 @@
         <v>67</v>
       </c>
       <c r="E26" s="40" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F26" s="34"/>
       <c r="G26" s="34"/>
@@ -3945,10 +3933,10 @@
         <v>100</v>
       </c>
       <c r="K26" s="35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L26" s="35" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="M26" s="35"/>
       <c r="N26" s="35"/>
@@ -3988,10 +3976,10 @@
         <v>100</v>
       </c>
       <c r="K27" s="35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L27" s="35" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="M27" s="35"/>
       <c r="N27" s="35"/>
@@ -4031,10 +4019,10 @@
         <v>100</v>
       </c>
       <c r="K28" s="35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L28" s="35" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="M28" s="35"/>
       <c r="N28" s="35"/>
@@ -4064,7 +4052,7 @@
         <v>72</v>
       </c>
       <c r="E29" s="40" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F29" s="34"/>
       <c r="G29" s="34"/>
@@ -4074,10 +4062,10 @@
         <v>100</v>
       </c>
       <c r="K29" s="35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L29" s="35" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="M29" s="35"/>
       <c r="N29" s="35"/>
@@ -4107,7 +4095,7 @@
         <v>73</v>
       </c>
       <c r="E30" s="40" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F30" s="34"/>
       <c r="G30" s="34"/>
@@ -4117,7 +4105,7 @@
         <v>100</v>
       </c>
       <c r="K30" s="35" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L30" s="35"/>
       <c r="M30" s="35"/>
@@ -4148,7 +4136,7 @@
         <v>74</v>
       </c>
       <c r="E31" s="40" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F31" s="34"/>
       <c r="G31" s="34"/>
@@ -4158,7 +4146,7 @@
         <v>100</v>
       </c>
       <c r="K31" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L31" s="35"/>
       <c r="M31" s="35"/>
@@ -4189,7 +4177,7 @@
         <v>75</v>
       </c>
       <c r="E32" s="40" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F32" s="34"/>
       <c r="G32" s="34"/>
@@ -4199,7 +4187,7 @@
         <v>100</v>
       </c>
       <c r="K32" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L32" s="35"/>
       <c r="M32" s="35"/>
@@ -4230,7 +4218,7 @@
         <v>76</v>
       </c>
       <c r="E33" s="40" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F33" s="34"/>
       <c r="G33" s="34"/>
@@ -4240,7 +4228,7 @@
         <v>100</v>
       </c>
       <c r="K33" s="35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L33" s="35"/>
       <c r="M33" s="35"/>
@@ -4271,7 +4259,7 @@
         <v>77</v>
       </c>
       <c r="E34" s="40" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F34" s="34"/>
       <c r="G34" s="34"/>
@@ -4281,7 +4269,7 @@
         <v>100</v>
       </c>
       <c r="K34" s="35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L34" s="35"/>
       <c r="M34" s="35"/>
@@ -4312,7 +4300,7 @@
         <v>78</v>
       </c>
       <c r="E35" s="40" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F35" s="34"/>
       <c r="G35" s="34"/>
@@ -4322,7 +4310,7 @@
         <v>100</v>
       </c>
       <c r="K35" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L35" s="35"/>
       <c r="M35" s="35"/>
@@ -4363,7 +4351,7 @@
         <v>100</v>
       </c>
       <c r="K36" s="35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L36" s="35"/>
       <c r="M36" s="35"/>
@@ -4404,7 +4392,7 @@
         <v>100</v>
       </c>
       <c r="K37" s="35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L37" s="35"/>
       <c r="M37" s="35"/>
@@ -4435,7 +4423,7 @@
         <v>83</v>
       </c>
       <c r="E38" s="40" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F38" s="34"/>
       <c r="G38" s="34"/>
@@ -4445,7 +4433,7 @@
         <v>100</v>
       </c>
       <c r="K38" s="35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L38" s="35"/>
       <c r="M38" s="35"/>
@@ -4476,7 +4464,7 @@
         <v>84</v>
       </c>
       <c r="E39" s="40" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F39" s="34"/>
       <c r="G39" s="34"/>
@@ -4486,7 +4474,7 @@
         <v>100</v>
       </c>
       <c r="K39" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L39" s="35"/>
       <c r="M39" s="35"/>
@@ -4517,7 +4505,7 @@
         <v>85</v>
       </c>
       <c r="E40" s="40" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F40" s="34"/>
       <c r="G40" s="34"/>
@@ -4527,7 +4515,7 @@
         <v>100</v>
       </c>
       <c r="K40" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L40" s="35"/>
       <c r="M40" s="35"/>
@@ -4558,7 +4546,7 @@
         <v>86</v>
       </c>
       <c r="E41" s="40" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F41" s="34"/>
       <c r="G41" s="34"/>
@@ -4568,10 +4556,10 @@
         <v>100</v>
       </c>
       <c r="K41" s="35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L41" s="35" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="M41" s="35"/>
       <c r="N41" s="35"/>
@@ -4601,7 +4589,7 @@
         <v>87</v>
       </c>
       <c r="E42" s="40" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F42" s="34"/>
       <c r="G42" s="34"/>
@@ -4611,10 +4599,10 @@
         <v>100</v>
       </c>
       <c r="K42" s="35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L42" s="35" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="M42" s="35"/>
       <c r="N42" s="35"/>
@@ -4644,7 +4632,7 @@
         <v>88</v>
       </c>
       <c r="E43" s="40" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F43" s="34"/>
       <c r="G43" s="34"/>
@@ -4654,10 +4642,10 @@
         <v>100</v>
       </c>
       <c r="K43" s="35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L43" s="35" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="M43" s="35"/>
       <c r="N43" s="35"/>
@@ -4687,7 +4675,7 @@
         <v>89</v>
       </c>
       <c r="E44" s="40" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F44" s="34"/>
       <c r="G44" s="34"/>
@@ -4697,10 +4685,10 @@
         <v>100</v>
       </c>
       <c r="K44" s="35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L44" s="35" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="M44" s="35"/>
       <c r="N44" s="35"/>
@@ -4730,7 +4718,7 @@
         <v>90</v>
       </c>
       <c r="E45" s="40" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F45" s="34"/>
       <c r="G45" s="34"/>
@@ -4740,7 +4728,7 @@
         <v>100</v>
       </c>
       <c r="K45" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L45" s="35"/>
       <c r="M45" s="35"/>
@@ -4771,7 +4759,7 @@
         <v>91</v>
       </c>
       <c r="E46" s="40" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F46" s="34"/>
       <c r="G46" s="34"/>
@@ -4781,7 +4769,7 @@
         <v>100</v>
       </c>
       <c r="K46" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L46" s="35"/>
       <c r="M46" s="35"/>
@@ -4809,22 +4797,22 @@
         <v>46</v>
       </c>
       <c r="D47" s="33" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E47" s="40" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F47" s="34">
         <v>45910</v>
       </c>
       <c r="G47" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="H47" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="I47" s="39" t="s">
         <v>190</v>
-      </c>
-      <c r="H47" s="34" t="s">
-        <v>192</v>
-      </c>
-      <c r="I47" s="39" t="s">
-        <v>193</v>
       </c>
       <c r="J47" s="35" t="s">
         <v>51</v>
@@ -4856,10 +4844,10 @@
         <v>46</v>
       </c>
       <c r="D48" s="33" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E48" s="40" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F48" s="34"/>
       <c r="G48" s="34"/>
@@ -4869,7 +4857,7 @@
         <v>100</v>
       </c>
       <c r="K48" s="35" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L48" s="35"/>
       <c r="M48" s="35"/>
@@ -4897,10 +4885,10 @@
         <v>46</v>
       </c>
       <c r="D49" s="33" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E49" s="40" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F49" s="33"/>
       <c r="G49" s="33"/>
@@ -4910,7 +4898,7 @@
         <v>100</v>
       </c>
       <c r="K49" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L49" s="33"/>
       <c r="M49" s="35"/>
@@ -4938,10 +4926,10 @@
         <v>38</v>
       </c>
       <c r="D50" s="33" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E50" s="40" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F50" s="33"/>
       <c r="G50" s="33"/>
@@ -4951,7 +4939,7 @@
         <v>100</v>
       </c>
       <c r="K50" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L50" s="33"/>
       <c r="M50" s="35"/>
@@ -4979,10 +4967,10 @@
         <v>46</v>
       </c>
       <c r="D51" s="33" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E51" s="40" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F51" s="33"/>
       <c r="G51" s="33"/>
@@ -4992,7 +4980,7 @@
         <v>100</v>
       </c>
       <c r="K51" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L51" s="33"/>
       <c r="M51" s="35"/>
@@ -5020,22 +5008,22 @@
         <v>38</v>
       </c>
       <c r="D52" s="33" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E52" s="40" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F52" s="34">
         <v>45910</v>
       </c>
       <c r="G52" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="H52" s="34" t="s">
         <v>191</v>
       </c>
-      <c r="H52" s="34" t="s">
-        <v>194</v>
-      </c>
       <c r="I52" s="39" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="J52" s="35" t="s">
         <v>51</v>
@@ -5067,10 +5055,10 @@
         <v>38</v>
       </c>
       <c r="D53" s="33" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E53" s="40" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F53" s="34"/>
       <c r="G53" s="34"/>
@@ -5080,7 +5068,7 @@
         <v>100</v>
       </c>
       <c r="K53" s="35" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L53" s="35"/>
       <c r="M53" s="35"/>
@@ -5108,10 +5096,10 @@
         <v>38</v>
       </c>
       <c r="D54" s="33" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E54" s="40" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F54" s="34"/>
       <c r="G54" s="34"/>
@@ -5121,7 +5109,7 @@
         <v>100</v>
       </c>
       <c r="K54" s="35" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L54" s="35"/>
       <c r="M54" s="35"/>
@@ -5149,10 +5137,10 @@
         <v>46</v>
       </c>
       <c r="D55" s="33" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E55" s="40" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F55" s="34"/>
       <c r="G55" s="34"/>
@@ -5162,7 +5150,7 @@
         <v>100</v>
       </c>
       <c r="K55" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L55" s="35"/>
       <c r="M55" s="35"/>
@@ -5181,7 +5169,7 @@
     </row>
     <row r="56" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F56" s="6"/>
-      <c r="G56" s="55"/>
+      <c r="G56" s="6"/>
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
       <c r="J56" s="7"/>
@@ -9213,23 +9201,23 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3DE61C5E-9DA3-4CE3-A1FF-8FBE651EA6B5}">
-          <x14:formula1>
-            <xm:f>'LISTA VALORI'!$A$2:$A$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>K49:K55 K10:K47</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{F5F4AC7B-142E-4F14-AD0B-95E75DB6B433}">
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J10:J55 P10:R55 M10:N55</xm:sqref>
+          <xm:sqref>P16:R55 M16:N55 M10:N13 P10:R13 J10:J55</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{70793024-27E9-4E6A-BACD-083AB683BC38}">
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>T10:T55</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3DE61C5E-9DA3-4CE3-A1FF-8FBE651EA6B5}">
+          <x14:formula1>
+            <xm:f>'LISTA VALORI'!$A$2:$A$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>K10:K55</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -9249,42 +9237,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -9298,7 +9286,7 @@
   <sheetViews>
     <sheetView zoomScale="106" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8:D8"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9314,7 +9302,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>15</v>
@@ -9326,10 +9314,10 @@
         <v>93</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9340,10 +9328,10 @@
         <v>94</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9354,10 +9342,10 @@
         <v>94</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9368,10 +9356,10 @@
         <v>94</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9382,10 +9370,10 @@
         <v>94</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9396,10 +9384,10 @@
         <v>94</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -9410,10 +9398,10 @@
         <v>94</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -9424,10 +9412,10 @@
         <v>94</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -9438,10 +9426,10 @@
         <v>94</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -9460,16 +9448,16 @@
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11492,15 +11480,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -11758,6 +11737,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
@@ -11776,14 +11764,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11802,6 +11782,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>